<commit_message>
PCA working with MLR, just numerical variables
</commit_message>
<xml_diff>
--- a/results/ML/DT_cEnroll_nPSU_nS1S2_vs_Desertor/backwardElimination.xlsx
+++ b/results/ML/DT_cEnroll_nPSU_nS1S2_vs_Desertor/backwardElimination.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\models\desertorstudent\results\ML\DT_cEnroll_nPSU_nS1S2_vs_Desertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87647C35-A607-429A-83E6-AFF2B39C2C64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5FB652-C6D4-4927-B034-C64B012830FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16800" yWindow="0" windowWidth="12000" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -208,7 +208,7 @@
 Model:                            OLS   Adj. R-squared:                  0.455
 Method:                 Least Squares   F-statistic:                     10.72
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           2.01e-49
-Time:                        14:27:12   Log-Likelihood:                -153.95
+Time:                        15:12:05   Log-Likelihood:                -153.95
 No. Observations:                 537   AIC:                             401.9
 Df Residuals:                     490   BIC:                             603.3
 Df Model:                          46                                         
@@ -281,7 +281,7 @@
 Model:                            OLS   Adj. R-squared:                  0.456
 Method:                 Least Squares   F-statistic:                     10.98
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           6.03e-50
-Time:                        14:27:12   Log-Likelihood:                -153.95
+Time:                        15:12:06   Log-Likelihood:                -153.95
 No. Observations:                 537   AIC:                             399.9
 Df Residuals:                     491   BIC:                             597.1
 Df Model:                          45                                         
@@ -353,7 +353,7 @@
 Model:                            OLS   Adj. R-squared:                  0.457
 Method:                 Least Squares   F-statistic:                     11.25
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           1.78e-50
-Time:                        14:27:12   Log-Likelihood:                -153.95
+Time:                        15:12:06   Log-Likelihood:                -153.95
 No. Observations:                 537   AIC:                             397.9
 Df Residuals:                     492   BIC:                             590.8
 Df Model:                          44                                         
@@ -424,7 +424,7 @@
 Model:                            OLS   Adj. R-squared:                  0.458
 Method:                 Least Squares   F-statistic:                     11.54
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           5.21e-51
-Time:                        14:27:12   Log-Likelihood:                -153.95
+Time:                        15:12:06   Log-Likelihood:                -153.95
 No. Observations:                 537   AIC:                             395.9
 Df Residuals:                     493   BIC:                             584.5
 Df Model:                          43                                         
@@ -494,7 +494,7 @@
 Model:                            OLS   Adj. R-squared:                  0.459
 Method:                 Least Squares   F-statistic:                     11.83
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           1.54e-51
-Time:                        14:27:12   Log-Likelihood:                -153.98
+Time:                        15:12:06   Log-Likelihood:                -153.98
 No. Observations:                 537   AIC:                             394.0
 Df Residuals:                     494   BIC:                             578.3
 Df Model:                          42                                         
@@ -563,7 +563,7 @@
 Model:                            OLS   Adj. R-squared:                  0.460
 Method:                 Least Squares   F-statistic:                     12.14
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           4.47e-52
-Time:                        14:27:12   Log-Likelihood:                -154.00
+Time:                        15:12:06   Log-Likelihood:                -154.00
 No. Observations:                 537   AIC:                             392.0
 Df Residuals:                     495   BIC:                             572.0
 Df Model:                          41                                         
@@ -631,7 +631,7 @@
 Model:                            OLS   Adj. R-squared:                  0.461
 Method:                 Least Squares   F-statistic:                     12.47
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           1.29e-52
-Time:                        14:27:12   Log-Likelihood:                -154.04
+Time:                        15:12:06   Log-Likelihood:                -154.04
 No. Observations:                 537   AIC:                             390.1
 Df Residuals:                     496   BIC:                             565.8
 Df Model:                          40                                         
@@ -698,7 +698,7 @@
 Model:                            OLS   Adj. R-squared:                  0.462
 Method:                 Least Squares   F-statistic:                     12.81
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           3.66e-53
-Time:                        14:27:12   Log-Likelihood:                -154.06
+Time:                        15:12:06   Log-Likelihood:                -154.06
 No. Observations:                 537   AIC:                             388.1
 Df Residuals:                     497   BIC:                             559.6
 Df Model:                          39                                         
@@ -764,7 +764,7 @@
 Model:                            OLS   Adj. R-squared:                  0.463
 Method:                 Least Squares   F-statistic:                     13.17
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           1.04e-53
-Time:                        14:27:12   Log-Likelihood:                -154.11
+Time:                        15:12:06   Log-Likelihood:                -154.11
 No. Observations:                 537   AIC:                             386.2
 Df Residuals:                     498   BIC:                             553.4
 Df Model:                          38                                         
@@ -829,7 +829,7 @@
 Model:                            OLS   Adj. R-squared:                  0.464
 Method:                 Least Squares   F-statistic:                     13.55
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           2.94e-54
-Time:                        14:27:12   Log-Likelihood:                -154.17
+Time:                        15:12:06   Log-Likelihood:                -154.17
 No. Observations:                 537   AIC:                             384.3
 Df Residuals:                     499   BIC:                             547.2
 Df Model:                          37                                         
@@ -893,7 +893,7 @@
 Model:                            OLS   Adj. R-squared:                  0.465
 Method:                 Least Squares   F-statistic:                     13.95
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           8.31e-55
-Time:                        14:27:12   Log-Likelihood:                -154.24
+Time:                        15:12:06   Log-Likelihood:                -154.24
 No. Observations:                 537   AIC:                             382.5
 Df Residuals:                     500   BIC:                             541.1
 Df Model:                          36                                         
@@ -956,7 +956,7 @@
 Model:                            OLS   Adj. R-squared:                  0.466
 Method:                 Least Squares   F-statistic:                     14.36
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           2.37e-55
-Time:                        14:27:12   Log-Likelihood:                -154.35
+Time:                        15:12:06   Log-Likelihood:                -154.35
 No. Observations:                 537   AIC:                             380.7
 Df Residuals:                     501   BIC:                             535.0
 Df Model:                          35                                         
@@ -1018,7 +1018,7 @@
 Model:                            OLS   Adj. R-squared:                  0.467
 Method:                 Least Squares   F-statistic:                     14.80
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           6.61e-56
-Time:                        14:27:12   Log-Likelihood:                -154.44
+Time:                        15:12:06   Log-Likelihood:                -154.44
 No. Observations:                 537   AIC:                             378.9
 Df Residuals:                     502   BIC:                             528.9
 Df Model:                          34                                         
@@ -1079,7 +1079,7 @@
 Model:                            OLS   Adj. R-squared:                  0.468
 Method:                 Least Squares   F-statistic:                     15.27
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           1.85e-56
-Time:                        14:27:12   Log-Likelihood:                -154.55
+Time:                        15:12:06   Log-Likelihood:                -154.55
 No. Observations:                 537   AIC:                             377.1
 Df Residuals:                     503   BIC:                             522.8
 Df Model:                          33                                         
@@ -1139,7 +1139,7 @@
 Model:                            OLS   Adj. R-squared:                  0.469
 Method:                 Least Squares   F-statistic:                     15.77
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           5.06e-57
-Time:                        14:27:12   Log-Likelihood:                -154.66
+Time:                        15:12:06   Log-Likelihood:                -154.66
 No. Observations:                 537   AIC:                             375.3
 Df Residuals:                     504   BIC:                             516.8
 Df Model:                          32                                         
@@ -1198,7 +1198,7 @@
 Model:                            OLS   Adj. R-squared:                  0.469
 Method:                 Least Squares   F-statistic:                     16.28
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           1.47e-57
-Time:                        14:27:12   Log-Likelihood:                -154.85
+Time:                        15:12:06   Log-Likelihood:                -154.85
 No. Observations:                 537   AIC:                             373.7
 Df Residuals:                     505   BIC:                             510.8
 Df Model:                          31                                         
@@ -1256,7 +1256,7 @@
 Model:                            OLS   Adj. R-squared:                  0.470
 Method:                 Least Squares   F-statistic:                     16.86
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           3.56e-58
-Time:                        14:27:12   Log-Likelihood:                -154.85
+Time:                        15:12:06   Log-Likelihood:                -154.85
 No. Observations:                 537   AIC:                             371.7
 Df Residuals:                     506   BIC:                             504.6
 Df Model:                          30                                         
@@ -1313,7 +1313,7 @@
 Model:                            OLS   Adj. R-squared:                  0.471
 Method:                 Least Squares   F-statistic:                     17.42
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           1.20e-58
-Time:                        14:27:12   Log-Likelihood:                -155.25
+Time:                        15:12:06   Log-Likelihood:                -155.25
 No. Observations:                 537   AIC:                             370.5
 Df Residuals:                     507   BIC:                             499.1
 Df Model:                          29                                         
@@ -1369,7 +1369,7 @@
 Model:                            OLS   Adj. R-squared:                  0.471
 Method:                 Least Squares   F-statistic:                     18.03
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           3.97e-59
-Time:                        14:27:12   Log-Likelihood:                -155.65
+Time:                        15:12:06   Log-Likelihood:                -155.65
 No. Observations:                 537   AIC:                             369.3
 Df Residuals:                     508   BIC:                             493.6
 Df Model:                          28                                         
@@ -1424,7 +1424,7 @@
 Model:                            OLS   Adj. R-squared:                  0.471
 Method:                 Least Squares   F-statistic:                     18.65
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           1.57e-59
-Time:                        14:27:12   Log-Likelihood:                -156.25
+Time:                        15:12:06   Log-Likelihood:                -156.25
 No. Observations:                 537   AIC:                             368.5
 Df Residuals:                     509   BIC:                             488.5
 Df Model:                          27                                         
@@ -1478,7 +1478,7 @@
 Model:                            OLS   Adj. R-squared:                  0.470
 Method:                 Least Squares   F-statistic:                     19.32
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           6.10e-60
-Time:                        14:27:12   Log-Likelihood:                -156.86
+Time:                        15:12:06   Log-Likelihood:                -156.86
 No. Observations:                 537   AIC:                             367.7
 Df Residuals:                     510   BIC:                             483.4
 Df Model:                          26                                         
@@ -1531,7 +1531,7 @@
 Model:                            OLS   Adj. R-squared:                  0.470
 Method:                 Least Squares   F-statistic:                     20.04
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           2.26e-60
-Time:                        14:27:12   Log-Likelihood:                -157.43
+Time:                        15:12:06   Log-Likelihood:                -157.43
 No. Observations:                 537   AIC:                             366.9
 Df Residuals:                     511   BIC:                             478.3
 Df Model:                          25                                         
@@ -1583,7 +1583,7 @@
 Model:                            OLS   Adj. R-squared:                  0.470
 Method:                 Least Squares   F-statistic:                     20.80
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           9.45e-61
-Time:                        14:27:12   Log-Likelihood:                -158.16
+Time:                        15:12:06   Log-Likelihood:                -158.16
 No. Observations:                 537   AIC:                             366.3
 Df Residuals:                     512   BIC:                             473.5
 Df Model:                          24                                         
@@ -1634,7 +1634,7 @@
 Model:                            OLS   Adj. R-squared:                  0.469
 Method:                 Least Squares   F-statistic:                     21.62
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           4.09e-61
-Time:                        14:27:13   Log-Likelihood:                -158.94
+Time:                        15:12:06   Log-Likelihood:                -158.94
 No. Observations:                 537   AIC:                             365.9
 Df Residuals:                     513   BIC:                             468.7
 Df Model:                          23                                         
@@ -1682,7 +1682,7 @@
 Model:                            OLS   Adj. R-squared:                  0.469
 Method:                 Least Squares   F-statistic:                     22.54
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           1.50e-61
-Time:                        14:27:13   Log-Likelihood:                -159.56
+Time:                        15:12:06   Log-Likelihood:                -159.56
 No. Observations:                 537   AIC:                             365.1
 Df Residuals:                     514   BIC:                             463.7
 Df Model:                          22                                         
@@ -1729,7 +1729,7 @@
 Model:                            OLS   Adj. R-squared:                  0.468
 Method:                 Least Squares   F-statistic:                     23.46
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           8.46e-62
-Time:                        14:27:13   Log-Likelihood:                -160.67
+Time:                        15:12:06   Log-Likelihood:                -160.67
 No. Observations:                 537   AIC:                             365.3
 Df Residuals:                     515   BIC:                             459.6
 Df Model:                          21                                         
@@ -1775,7 +1775,7 @@
 Model:                            OLS   Adj. R-squared:                  0.467
 Method:                 Least Squares   F-statistic:                     24.45
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           5.22e-62
-Time:                        14:27:13   Log-Likelihood:                -161.90
+Time:                        15:12:06   Log-Likelihood:                -161.90
 No. Observations:                 537   AIC:                             365.8
 Df Residuals:                     516   BIC:                             455.8
 Df Model:                          20                                         
@@ -1820,7 +1820,7 @@
 Model:                            OLS   Adj. R-squared:                  0.464
 Method:                 Least Squares   F-statistic:                     25.45
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           4.94e-62
-Time:                        14:27:13   Log-Likelihood:                -163.60
+Time:                        15:12:06   Log-Likelihood:                -163.60
 No. Observations:                 537   AIC:                             367.2
 Df Residuals:                     517   BIC:                             452.9
 Df Model:                          19                                         
@@ -1864,7 +1864,7 @@
 Model:                            OLS   Adj. R-squared:                  0.464
 Method:                 Least Squares   F-statistic:                     26.81
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           1.57e-62
-Time:                        14:27:13   Log-Likelihood:                -164.16
+Time:                        15:12:06   Log-Likelihood:                -164.16
 No. Observations:                 537   AIC:                             366.3
 Df Residuals:                     518   BIC:                             447.8
 Df Model:                          18                                         
@@ -1907,7 +1907,7 @@
 Model:                            OLS   Adj. R-squared:                  0.464
 Method:                 Least Squares   F-statistic:                     28.34
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           4.34e-63
-Time:                        14:27:13   Log-Likelihood:                -164.59
+Time:                        15:12:06   Log-Likelihood:                -164.59
 No. Observations:                 537   AIC:                             365.2
 Df Residuals:                     519   BIC:                             442.3
 Df Model:                          17                                         
@@ -1949,7 +1949,7 @@
 Model:                            OLS   Adj. R-squared:                  0.464
 Method:                 Least Squares   F-statistic:                     30.02
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           1.42e-63
-Time:                        14:27:13   Log-Likelihood:                -165.24
+Time:                        15:12:06   Log-Likelihood:                -165.24
 No. Observations:                 537   AIC:                             364.5
 Df Residuals:                     520   BIC:                             437.3
 Df Model:                          16                                         
@@ -1990,7 +1990,7 @@
 Model:                            OLS   Adj. R-squared:                  0.464
 Method:                 Least Squares   F-statistic:                     31.94
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           4.20e-64
-Time:                        14:27:13   Log-Likelihood:                -165.80
+Time:                        15:12:06   Log-Likelihood:                -165.80
 No. Observations:                 537   AIC:                             363.6
 Df Residuals:                     521   BIC:                             432.2
 Df Model:                          15                                         
@@ -2030,7 +2030,7 @@
 Model:                            OLS   Adj. R-squared:                  0.463
 Method:                 Least Squares   F-statistic:                     34.06
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           1.59e-64
-Time:                        14:27:13   Log-Likelihood:                -166.66
+Time:                        15:12:06   Log-Likelihood:                -166.66
 No. Observations:                 537   AIC:                             363.3
 Df Residuals:                     522   BIC:                             427.6
 Df Model:                          14                                         
@@ -2069,7 +2069,7 @@
 Model:                            OLS   Adj. R-squared:                  0.462
 Method:                 Least Squares   F-statistic:                     36.46
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           6.74e-65
-Time:                        14:27:13   Log-Likelihood:                -167.68
+Time:                        15:12:06   Log-Likelihood:                -167.68
 No. Observations:                 537   AIC:                             363.4
 Df Residuals:                     523   BIC:                             423.4
 Df Model:                          13                                         
@@ -2107,7 +2107,7 @@
 Model:                            OLS   Adj. R-squared:                  0.460
 Method:                 Least Squares   F-statistic:                     39.10
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           4.58e-65
-Time:                        14:27:13   Log-Likelihood:                -169.22
+Time:                        15:12:06   Log-Likelihood:                -169.22
 No. Observations:                 537   AIC:                             364.4
 Df Residuals:                     524   BIC:                             420.2
 Df Model:                          12                                         
@@ -2144,7 +2144,7 @@
 Model:                            OLS   Adj. R-squared:                  0.459
 Method:                 Least Squares   F-statistic:                     42.27
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           2.59e-65
-Time:                        14:27:13   Log-Likelihood:                -170.61
+Time:                        15:12:06   Log-Likelihood:                -170.61
 No. Observations:                 537   AIC:                             365.2
 Df Residuals:                     525   BIC:                             416.7
 Df Model:                          11                                         
@@ -2180,7 +2180,7 @@
 Model:                            OLS   Adj. R-squared:                  0.456
 Method:                 Least Squares   F-statistic:                     45.97
 Date:                Wed, 25 Dec 2019   Prob (F-statistic):           1.85e-65
-Time:                        14:27:13   Log-Likelihood:                -172.29
+Time:                        15:12:06   Log-Likelihood:                -172.29
 No. Observations:                 537   AIC:                             366.6
 Df Residuals:                     526   BIC:                             413.7
 Df Model:                          10                                         

</xml_diff>

<commit_message>
added excel file of mlr dt trainings
</commit_message>
<xml_diff>
--- a/results/ML/DT_cEnroll_nPSU_nS1S2_vs_Desertor/backwardElimination.xlsx
+++ b/results/ML/DT_cEnroll_nPSU_nS1S2_vs_Desertor/backwardElimination.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\models\desertorstudent\results\ML\DT_cEnroll_nPSU_nS1S2_vs_Desertor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Reference\models\desertorstudent\results\ML\DT_cEnroll_nPSU_nS1S2_vs_Desertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD01818-1822-4548-B80A-28F6A6E1D09F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C856D85-CCE4-4C06-8C2C-5799C9C775B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16800" yWindow="0" windowWidth="12000" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -199,8 +199,8 @@
 Dep. Variable:               Desertor   R-squared:                       0.502
 Model:                            OLS   Adj. R-squared:                  0.455
 Method:                 Least Squares   F-statistic:                     10.72
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):           2.01e-49
-Time:                        20:59:55   Log-Likelihood:                -153.95
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):           2.01e-49
+Time:                        16:11:27   Log-Likelihood:                -153.95
 No. Observations:                 537   AIC:                             401.9
 Df Residuals:                     490   BIC:                             603.3
 Df Model:                          46                                         
@@ -272,8 +272,8 @@
 Dep. Variable:               Desertor   R-squared:                       0.502
 Model:                            OLS   Adj. R-squared:                  0.456
 Method:                 Least Squares   F-statistic:                     10.98
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):           6.03e-50
-Time:                        20:59:55   Log-Likelihood:                -153.95
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):           6.03e-50
+Time:                        16:11:27   Log-Likelihood:                -153.95
 No. Observations:                 537   AIC:                             399.9
 Df Residuals:                     491   BIC:                             597.1
 Df Model:                          45                                         
@@ -344,8 +344,8 @@
 Dep. Variable:               Desertor   R-squared:                       0.502
 Model:                            OLS   Adj. R-squared:                  0.457
 Method:                 Least Squares   F-statistic:                     11.25
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):           1.78e-50
-Time:                        20:59:55   Log-Likelihood:                -153.95
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):           1.78e-50
+Time:                        16:11:27   Log-Likelihood:                -153.95
 No. Observations:                 537   AIC:                             397.9
 Df Residuals:                     492   BIC:                             590.8
 Df Model:                          44                                         
@@ -415,8 +415,8 @@
 Dep. Variable:               Desertor   R-squared:                       0.502
 Model:                            OLS   Adj. R-squared:                  0.458
 Method:                 Least Squares   F-statistic:                     11.54
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):           5.22e-51
-Time:                        20:59:55   Log-Likelihood:                -153.95
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):           5.22e-51
+Time:                        16:11:27   Log-Likelihood:                -153.95
 No. Observations:                 537   AIC:                             395.9
 Df Residuals:                     493   BIC:                             584.5
 Df Model:                          43                                         
@@ -485,8 +485,8 @@
 Dep. Variable:               Desertor   R-squared:                       0.502
 Model:                            OLS   Adj. R-squared:                  0.459
 Method:                 Least Squares   F-statistic:                     11.84
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):           1.51e-51
-Time:                        20:59:55   Log-Likelihood:                -153.95
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):           1.51e-51
+Time:                        16:11:27   Log-Likelihood:                -153.95
 No. Observations:                 537   AIC:                             393.9
 Df Residuals:                     494   BIC:                             578.2
 Df Model:                          42                                         
@@ -554,8 +554,8 @@
 Dep. Variable:               Desertor   R-squared:                       0.502
 Model:                            OLS   Adj. R-squared:                  0.460
 Method:                 Least Squares   F-statistic:                     12.15
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):           4.31e-52
-Time:                        20:59:55   Log-Likelihood:                -153.96
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):           4.31e-52
+Time:                        16:11:27   Log-Likelihood:                -153.96
 No. Observations:                 537   AIC:                             391.9
 Df Residuals:                     495   BIC:                             571.9
 Df Model:                          41                                         
@@ -622,8 +622,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.649
 Model:                            OLS   Adj. R-squared (uncentered):              0.620
 Method:                 Least Squares   F-statistic:                              22.38
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    7.29e-88
-Time:                        20:59:55   Log-Likelihood:                         -153.99
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    7.29e-88
+Time:                        16:11:27   Log-Likelihood:                         -153.99
 No. Observations:                 537   AIC:                                      390.0
 Df Residuals:                     496   BIC:                                      565.7
 Df Model:                          41                                                  
@@ -689,8 +689,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.649
 Model:                            OLS   Adj. R-squared (uncentered):              0.621
 Method:                 Least Squares   F-statistic:                              22.98
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    1.53e-88
-Time:                        20:59:55   Log-Likelihood:                         -154.01
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    1.53e-88
+Time:                        16:11:27   Log-Likelihood:                         -154.01
 No. Observations:                 537   AIC:                                      388.0
 Df Residuals:                     497   BIC:                                      559.5
 Df Model:                          40                                                  
@@ -755,8 +755,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.649
 Model:                            OLS   Adj. R-squared (uncentered):              0.622
 Method:                 Least Squares   F-statistic:                              23.61
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    3.22e-89
-Time:                        20:59:56   Log-Likelihood:                         -154.04
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    3.22e-89
+Time:                        16:11:27   Log-Likelihood:                         -154.04
 No. Observations:                 537   AIC:                                      386.1
 Df Residuals:                     498   BIC:                                      553.2
 Df Model:                          39                                                  
@@ -820,8 +820,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.649
 Model:                            OLS   Adj. R-squared (uncentered):              0.622
 Method:                 Least Squares   F-statistic:                              24.28
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    6.53e-90
-Time:                        20:59:56   Log-Likelihood:                         -154.05
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    6.53e-90
+Time:                        16:11:27   Log-Likelihood:                         -154.05
 No. Observations:                 537   AIC:                                      384.1
 Df Residuals:                     499   BIC:                                      547.0
 Df Model:                          38                                                  
@@ -884,8 +884,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.649
 Model:                            OLS   Adj. R-squared (uncentered):              0.623
 Method:                 Least Squares   F-statistic:                              24.99
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    1.33e-90
-Time:                        20:59:56   Log-Likelihood:                         -154.08
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    1.33e-90
+Time:                        16:11:27   Log-Likelihood:                         -154.08
 No. Observations:                 537   AIC:                                      382.2
 Df Residuals:                     500   BIC:                                      540.7
 Df Model:                          37                                                  
@@ -947,8 +947,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.649
 Model:                            OLS   Adj. R-squared (uncentered):              0.624
 Method:                 Least Squares   F-statistic:                              25.73
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    2.69e-91
-Time:                        20:59:56   Log-Likelihood:                         -154.12
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    2.69e-91
+Time:                        16:11:27   Log-Likelihood:                         -154.12
 No. Observations:                 537   AIC:                                      380.2
 Df Residuals:                     501   BIC:                                      534.5
 Df Model:                          36                                                  
@@ -1009,8 +1009,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.649
 Model:                            OLS   Adj. R-squared (uncentered):              0.624
 Method:                 Least Squares   F-statistic:                              26.51
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    5.36e-92
-Time:                        20:59:56   Log-Likelihood:                         -154.15
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    5.36e-92
+Time:                        16:11:27   Log-Likelihood:                         -154.15
 No. Observations:                 537   AIC:                                      378.3
 Df Residuals:                     502   BIC:                                      528.3
 Df Model:                          35                                                  
@@ -1070,8 +1070,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.649
 Model:                            OLS   Adj. R-squared (uncentered):              0.625
 Method:                 Least Squares   F-statistic:                              27.33
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    1.07e-92
-Time:                        20:59:56   Log-Likelihood:                         -154.21
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    1.07e-92
+Time:                        16:11:27   Log-Likelihood:                         -154.21
 No. Observations:                 537   AIC:                                      376.4
 Df Residuals:                     503   BIC:                                      522.1
 Df Model:                          34                                                  
@@ -1130,8 +1130,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.649
 Model:                            OLS   Adj. R-squared (uncentered):              0.626
 Method:                 Least Squares   F-statistic:                              28.21
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    2.11e-93
-Time:                        20:59:56   Log-Likelihood:                         -154.27
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    2.11e-93
+Time:                        16:11:27   Log-Likelihood:                         -154.27
 No. Observations:                 537   AIC:                                      374.5
 Df Residuals:                     504   BIC:                                      516.0
 Df Model:                          33                                                  
@@ -1189,8 +1189,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.649
 Model:                            OLS   Adj. R-squared (uncentered):              0.626
 Method:                 Least Squares   F-statistic:                              29.13
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    4.23e-94
-Time:                        20:59:56   Log-Likelihood:                         -154.37
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    4.23e-94
+Time:                        16:11:27   Log-Likelihood:                         -154.37
 No. Observations:                 537   AIC:                                      372.7
 Df Residuals:                     505   BIC:                                      509.9
 Df Model:                          32                                                  
@@ -1247,8 +1247,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.648
 Model:                            OLS   Adj. R-squared (uncentered):              0.627
 Method:                 Least Squares   F-statistic:                              30.11
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    8.41e-95
-Time:                        20:59:56   Log-Likelihood:                         -154.48
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    8.41e-95
+Time:                        16:11:27   Log-Likelihood:                         -154.48
 No. Observations:                 537   AIC:                                      371.0
 Df Residuals:                     506   BIC:                                      503.8
 Df Model:                          31                                                  
@@ -1304,8 +1304,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.648
 Model:                            OLS   Adj. R-squared (uncentered):              0.627
 Method:                 Least Squares   F-statistic:                              31.15
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    1.67e-95
-Time:                        20:59:56   Log-Likelihood:                         -154.60
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    1.67e-95
+Time:                        16:11:27   Log-Likelihood:                         -154.60
 No. Observations:                 537   AIC:                                      369.2
 Df Residuals:                     507   BIC:                                      497.8
 Df Model:                          30                                                  
@@ -1360,8 +1360,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.648
 Model:                            OLS   Adj. R-squared (uncentered):              0.628
 Method:                 Least Squares   F-statistic:                              32.27
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    3.27e-96
-Time:                        20:59:56   Log-Likelihood:                         -154.73
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    3.27e-96
+Time:                        16:11:27   Log-Likelihood:                         -154.73
 No. Observations:                 537   AIC:                                      367.5
 Df Residuals:                     508   BIC:                                      491.7
 Df Model:                          29                                                  
@@ -1415,8 +1415,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.648
 Model:                            OLS   Adj. R-squared (uncentered):              0.628
 Method:                 Least Squares   F-statistic:                              33.44
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    7.05e-97
-Time:                        20:59:56   Log-Likelihood:                         -154.98
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    7.05e-97
+Time:                        16:11:27   Log-Likelihood:                         -154.98
 No. Observations:                 537   AIC:                                      366.0
 Df Residuals:                     509   BIC:                                      486.0
 Df Model:                          28                                                  
@@ -1469,8 +1469,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.647
 Model:                            OLS   Adj. R-squared (uncentered):              0.629
 Method:                 Least Squares   F-statistic:                              34.69
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    1.53e-97
-Time:                        20:59:56   Log-Likelihood:                         -155.25
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    1.53e-97
+Time:                        16:11:27   Log-Likelihood:                         -155.25
 No. Observations:                 537   AIC:                                      364.5
 Df Residuals:                     510   BIC:                                      480.2
 Df Model:                          27                                                  
@@ -1522,8 +1522,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.647
 Model:                            OLS   Adj. R-squared (uncentered):              0.629
 Method:                 Least Squares   F-statistic:                              36.05
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    3.04e-98
-Time:                        20:59:56   Log-Likelihood:                         -155.46
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    3.04e-98
+Time:                        16:11:27   Log-Likelihood:                         -155.46
 No. Observations:                 537   AIC:                                      362.9
 Df Residuals:                     511   BIC:                                      474.4
 Df Model:                          26                                                  
@@ -1574,8 +1574,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.647
 Model:                            OLS   Adj. R-squared (uncentered):              0.630
 Method:                 Least Squares   F-statistic:                              37.56
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    5.05e-99
-Time:                        20:59:56   Log-Likelihood:                         -155.49
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    5.05e-99
+Time:                        16:11:27   Log-Likelihood:                         -155.49
 No. Observations:                 537   AIC:                                      361.0
 Df Residuals:                     512   BIC:                                      468.1
 Df Model:                          25                                                  
@@ -1625,8 +1625,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.647
 Model:                            OLS   Adj. R-squared (uncentered):              0.630
 Method:                 Least Squares   F-statistic:                              39.12
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    1.13e-99
-Time:                        20:59:56   Log-Likelihood:                         -155.87
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                    1.13e-99
+Time:                        16:11:28   Log-Likelihood:                         -155.87
 No. Observations:                 537   AIC:                                      359.7
 Df Residuals:                     513   BIC:                                      462.6
 Df Model:                          24                                                  
@@ -1675,8 +1675,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.646
 Model:                            OLS   Adj. R-squared (uncentered):              0.630
 Method:                 Least Squares   F-statistic:                              40.79
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                   2.71e-100
-Time:                        20:59:56   Log-Likelihood:                         -156.33
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                   2.71e-100
+Time:                        16:11:28   Log-Likelihood:                         -156.33
 No. Observations:                 537   AIC:                                      358.7
 Df Residuals:                     514   BIC:                                      457.2
 Df Model:                          23                                                  
@@ -1724,8 +1724,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.645
 Model:                            OLS   Adj. R-squared (uncentered):              0.630
 Method:                 Least Squares   F-statistic:                              42.56
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                   7.59e-101
-Time:                        20:59:56   Log-Likelihood:                         -156.99
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                   7.59e-101
+Time:                        16:11:28   Log-Likelihood:                         -156.99
 No. Observations:                 537   AIC:                                      358.0
 Df Residuals:                     515   BIC:                                      452.3
 Df Model:                          22                                                  
@@ -1772,8 +1772,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.644
 Model:                            OLS   Adj. R-squared (uncentered):              0.630
 Method:                 Least Squares   F-statistic:                              44.50
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                   2.16e-101
-Time:                        20:59:56   Log-Likelihood:                         -157.69
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                   2.16e-101
+Time:                        16:11:28   Log-Likelihood:                         -157.69
 No. Observations:                 537   AIC:                                      357.4
 Df Residuals:                     516   BIC:                                      447.4
 Df Model:                          21                                                  
@@ -1819,8 +1819,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.643
 Model:                            OLS   Adj. R-squared (uncentered):              0.629
 Method:                 Least Squares   F-statistic:                              46.61
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                   6.25e-102
-Time:                        20:59:56   Log-Likelihood:                         -158.43
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                   6.25e-102
+Time:                        16:11:28   Log-Likelihood:                         -158.43
 No. Observations:                 537   AIC:                                      356.9
 Df Residuals:                     517   BIC:                                      442.6
 Df Model:                          20                                                  
@@ -1865,8 +1865,8 @@
 Dep. Variable:               Desertor   R-squared (uncentered):                   0.640
 Model:                            OLS   Adj. R-squared (uncentered):              0.627
 Method:                 Least Squares   F-statistic:                              51.23
-Date:                Sat, 28 Dec 2019   Prob (F-statistic):                   1.33e-102
-Time:                        20:59:56   Log-Likelihood:                         -160.96
+Date:                Sun, 29 Dec 2019   Prob (F-statistic):                   1.33e-102
+Time:                        16:11:28   Log-Likelihood:                         -160.96
 No. Observations:                 537   AIC:                                      357.9
 Df Residuals:                     519   BIC:                                      435.1
 Df Model:                          18                                                  

</xml_diff>